<commit_message>
added all 21/22 for energy
</commit_message>
<xml_diff>
--- a/reporte_estadistico/data/energia/metricsCategorias/metrics_21/cat1/metrics_data_pfac.xlsx
+++ b/reporte_estadistico/data/energia/metricsCategorias/metrics_21/cat1/metrics_data_pfac.xlsx
@@ -1,21 +1,91 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\JJ\repos\research_eslatina\reporte_estadistico\data\energia\metricsCategorias\metrics_21\cat1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="236" yWindow="13" windowWidth="16089" windowHeight="9661"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>quant0</t>
+  </si>
+  <si>
+    <t>quant25</t>
+  </si>
+  <si>
+    <t>quant50</t>
+  </si>
+  <si>
+    <t>quant75</t>
+  </si>
+  <si>
+    <t>quant100</t>
+  </si>
+  <si>
+    <t>skewness</t>
+  </si>
+  <si>
+    <t>kurtosis</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>std_dev</t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Estrato1_pfac</t>
+  </si>
+  <si>
+    <t>Estrato2_pfac</t>
+  </si>
+  <si>
+    <t>Estrato3_pfac</t>
+  </si>
+  <si>
+    <t>Estrato4_pfac</t>
+  </si>
+  <si>
+    <t>Estrato5_pfac</t>
+  </si>
+  <si>
+    <t>Estrato6_pfac</t>
+  </si>
+  <si>
+    <t>totResidencial_pfac</t>
+  </si>
+  <si>
+    <t>totNoResidencial_pfac</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,11 +133,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +187,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +219,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +254,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,80 +430,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>quant0</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>quant25</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>quant50</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>quant75</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>quant100</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>skewness</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>kurtosis</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>median</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>std_dev</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>variance</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Estrato1_pfac</t>
-        </is>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2">
         <v>8.349099166666667</v>
@@ -432,50 +486,48 @@
         <v>24.8152128125</v>
       </c>
       <c r="D2">
-        <v>35.87302625</v>
+        <v>35.873026250000002</v>
       </c>
       <c r="E2">
-        <v>50.83582056818182</v>
+        <v>50.835820568181823</v>
       </c>
       <c r="F2">
-        <v>7094.083295833333</v>
+        <v>7094.0832958333331</v>
       </c>
       <c r="G2">
-        <v>4.40945229143019</v>
+        <v>4.4094522914301901</v>
       </c>
       <c r="H2">
         <v>30.63035541731039</v>
       </c>
       <c r="I2">
-        <v>35.87302625</v>
+        <v>35.873026250000002</v>
       </c>
       <c r="J2">
-        <v>543.7179931044099</v>
+        <v>543.71799310440986</v>
       </c>
       <c r="K2">
-        <v>295629.2560254871</v>
+        <v>295629.25602548709</v>
       </c>
       <c r="L2">
         <v>103.7202843502244</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Estrato2_pfac</t>
-        </is>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>13.80008083333333</v>
+        <v>13.800080833333331</v>
       </c>
       <c r="C3">
         <v>28.72580270833333</v>
       </c>
       <c r="D3">
-        <v>39.08018250000001</v>
+        <v>39.080182500000006</v>
       </c>
       <c r="E3">
-        <v>54.30036208333333</v>
+        <v>54.300362083333333</v>
       </c>
       <c r="F3">
         <v>998.7744183333333</v>
@@ -484,106 +536,100 @@
         <v>6.948820565653417</v>
       </c>
       <c r="H3">
-        <v>68.45299202722113</v>
+        <v>68.452992027221129</v>
       </c>
       <c r="I3">
-        <v>39.08018250000001</v>
+        <v>39.080182500000006</v>
       </c>
       <c r="J3">
-        <v>99.02311046505174</v>
+        <v>99.023110465051744</v>
       </c>
       <c r="K3">
         <v>9805.576406173841</v>
       </c>
       <c r="L3">
-        <v>58.31537146219336</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Estrato3_pfac</t>
-        </is>
+        <v>58.315371462193362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>33.17504937499999</v>
+        <v>33.175049374999993</v>
       </c>
       <c r="D4">
-        <v>55.14237041666667</v>
+        <v>55.142370416666672</v>
       </c>
       <c r="E4">
-        <v>76.56426</v>
+        <v>76.564260000000004</v>
       </c>
       <c r="F4">
-        <v>932.7314583333334</v>
+        <v>932.73145833333342</v>
       </c>
       <c r="G4">
         <v>3.798309654118023</v>
       </c>
       <c r="H4">
-        <v>25.66451380568404</v>
+        <v>25.664513805684042</v>
       </c>
       <c r="I4">
-        <v>55.14237041666667</v>
+        <v>55.142370416666672</v>
       </c>
       <c r="J4">
         <v>105.4914953209901</v>
       </c>
       <c r="K4">
-        <v>11128.45558505847</v>
+        <v>11128.455585058469</v>
       </c>
       <c r="L4">
-        <v>77.4012898377451</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Estrato4_pfac</t>
-        </is>
+        <v>77.401289837745097</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>26.73642636363637</v>
+        <v>26.736426363636369</v>
       </c>
       <c r="D5">
-        <v>71.52339916666666</v>
+        <v>71.523399166666664</v>
       </c>
       <c r="E5">
-        <v>139.745875</v>
+        <v>139.74587500000001</v>
       </c>
       <c r="F5">
-        <v>461.0951845833333</v>
+        <v>461.09518458333332</v>
       </c>
       <c r="G5">
-        <v>1.246592118656695</v>
+        <v>1.2465921186566951</v>
       </c>
       <c r="H5">
         <v>3.984471202139177</v>
       </c>
       <c r="I5">
-        <v>71.52339916666666</v>
+        <v>71.523399166666664</v>
       </c>
       <c r="J5">
-        <v>94.68743146423864</v>
+        <v>94.687431464238642</v>
       </c>
       <c r="K5">
-        <v>8965.70967729489</v>
+        <v>8965.7096772948898</v>
       </c>
       <c r="L5">
-        <v>96.60068765755379</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Estrato5_pfac</t>
-        </is>
+        <v>96.600687657553792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
       </c>
       <c r="B6">
         <v>-132.7572222222222</v>
@@ -592,38 +638,36 @@
         <v>28.47637125</v>
       </c>
       <c r="D6">
-        <v>76.22940249999999</v>
+        <v>76.229402499999992</v>
       </c>
       <c r="E6">
-        <v>140.32967</v>
+        <v>140.32966999999999</v>
       </c>
       <c r="F6">
         <v>3033.4</v>
       </c>
       <c r="G6">
-        <v>0.9715156328451464</v>
+        <v>0.97151563284514642</v>
       </c>
       <c r="H6">
-        <v>3.230876799790453</v>
+        <v>3.2308767997904528</v>
       </c>
       <c r="I6">
-        <v>76.22940249999999</v>
+        <v>76.229402499999992</v>
       </c>
       <c r="J6">
-        <v>621.3931644547433</v>
+        <v>621.39316445474333</v>
       </c>
       <c r="K6">
-        <v>386129.4648310797</v>
+        <v>386129.46483107971</v>
       </c>
       <c r="L6">
         <v>213.1741991820378</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Estrato6_pfac</t>
-        </is>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -632,111 +676,107 @@
         <v>62.6965</v>
       </c>
       <c r="D7">
-        <v>143.95575</v>
+        <v>143.95574999999999</v>
       </c>
       <c r="E7">
-        <v>304.857375</v>
+        <v>304.85737499999999</v>
       </c>
       <c r="F7">
-        <v>857.253375</v>
+        <v>857.25337500000001</v>
       </c>
       <c r="G7">
-        <v>0.9148133586550062</v>
+        <v>0.91481335865500624</v>
       </c>
       <c r="H7">
         <v>2.691864703425801</v>
       </c>
       <c r="I7">
-        <v>143.95575</v>
+        <v>143.95574999999999</v>
       </c>
       <c r="J7">
-        <v>223.9163372504918</v>
+        <v>223.91633725049181</v>
       </c>
       <c r="K7">
-        <v>50138.52608767598</v>
+        <v>50138.526087675978</v>
       </c>
       <c r="L7">
         <v>222.2703491233766</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>totResidencial_pfac</t>
-        </is>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
       <c r="B8">
         <v>14.89652166666667</v>
       </c>
       <c r="C8">
-        <v>28.31601458333334</v>
+        <v>28.316014583333342</v>
       </c>
       <c r="D8">
-        <v>38.10120208333333</v>
+        <v>38.101202083333327</v>
       </c>
       <c r="E8">
-        <v>52.83725687499999</v>
+        <v>52.837256874999987</v>
       </c>
       <c r="F8">
-        <v>6648.8598525</v>
+        <v>6648.8598524999998</v>
       </c>
       <c r="G8">
-        <v>5.218074819767757</v>
+        <v>5.2180748197677573</v>
       </c>
       <c r="H8">
-        <v>37.64026949443748</v>
+        <v>37.640269494437483</v>
       </c>
       <c r="I8">
-        <v>38.10120208333333</v>
+        <v>38.101202083333327</v>
       </c>
       <c r="J8">
-        <v>514.885884130154</v>
+        <v>514.88588413015395</v>
       </c>
       <c r="K8">
-        <v>265107.4736764903</v>
+        <v>265107.47367649031</v>
       </c>
       <c r="L8">
-        <v>105.4861229958236</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>totNoResidencial_pfac</t>
-        </is>
+        <v>105.48612299582361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
       </c>
       <c r="B9">
-        <v>16.25701818181818</v>
+        <v>16.257018181818179</v>
       </c>
       <c r="C9">
-        <v>150.32698125</v>
+        <v>150.32698124999999</v>
       </c>
       <c r="D9">
-        <v>200.2499679166667</v>
+        <v>200.24996791666669</v>
       </c>
       <c r="E9">
-        <v>322.5716925</v>
+        <v>322.57169249999998</v>
       </c>
       <c r="F9">
-        <v>1696.652116666667</v>
+        <v>1696.6521166666671</v>
       </c>
       <c r="G9">
-        <v>2.404406613285683</v>
+        <v>2.4044066132856829</v>
       </c>
       <c r="H9">
         <v>10.18828644237931</v>
       </c>
       <c r="I9">
-        <v>200.2499679166667</v>
+        <v>200.24996791666669</v>
       </c>
       <c r="J9">
         <v>241.8670485043402</v>
       </c>
       <c r="K9">
-        <v>58499.66915220088</v>
+        <v>58499.669152200877</v>
       </c>
       <c r="L9">
-        <v>280.7704366015755</v>
+        <v>280.77043660157551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>